<commit_message>
Change A Wave math
</commit_message>
<xml_diff>
--- a/Wave Math/Tone_calculator.xlsx
+++ b/Wave Math/Tone_calculator.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Base tone" sheetId="1" r:id="rId1"/>
     <sheet name="A4" sheetId="2" r:id="rId2"/>
-    <sheet name="C5" sheetId="3" r:id="rId3"/>
-    <sheet name="E5" sheetId="4" r:id="rId4"/>
-    <sheet name="Chord Test" sheetId="5" r:id="rId5"/>
+    <sheet name="A4 test" sheetId="6" r:id="rId3"/>
+    <sheet name="C5" sheetId="3" r:id="rId4"/>
+    <sheet name="E5" sheetId="4" r:id="rId5"/>
+    <sheet name="Chord Test" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
   <si>
     <t>step (binary)</t>
   </si>
@@ -983,11 +984,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="463687208"/>
-        <c:axId val="463682896"/>
+        <c:axId val="433611592"/>
+        <c:axId val="433613552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="463687208"/>
+        <c:axId val="433611592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1044,12 +1045,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463682896"/>
+        <c:crossAx val="433613552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="463682896"/>
+        <c:axId val="433613552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,7 +1107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463687208"/>
+        <c:crossAx val="433611592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3723,8 +3724,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="463683680"/>
-        <c:axId val="463684464"/>
+        <c:axId val="433613944"/>
+        <c:axId val="433614728"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -4472,7 +4473,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="463683680"/>
+        <c:axId val="433613944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4528,12 +4529,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463684464"/>
+        <c:crossAx val="433614728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="463684464"/>
+        <c:axId val="433614728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4590,7 +4591,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463683680"/>
+        <c:crossAx val="433613944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6087,7 +6088,7 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7703,8 +7704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H111"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8069,6 +8070,13 @@
         <f t="shared" si="3"/>
         <v>0001001</v>
       </c>
+      <c r="M11">
+        <v>30820</v>
+      </c>
+      <c r="N11">
+        <f>M11*0.000001</f>
+        <v>3.082E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -11076,6 +11084,2369 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>1/48000*A2 *1000</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>SIN(RADIANS(D2))</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>IF(E2&gt;=0, E2*32767, E2*32767+32767*2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <f>DEC2HEX(F2, 4)</f>
+        <v>0000</v>
+      </c>
+      <c r="H2" t="str">
+        <f>DEC2BIN(A2,7)</f>
+        <v>0000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>B2+0.03082</f>
+        <v>3.082E-2</v>
+      </c>
+      <c r="D3">
+        <f>D2+360/75</f>
+        <v>4.8</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="0">SIN(RADIANS(D3))</f>
+        <v>8.3677843332315482E-2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="1">IF(E3&gt;=0, E3*32767, E3*32767+32767*2)</f>
+        <v>2741.8718924699815</v>
+      </c>
+      <c r="G3" t="str">
+        <f>DEC2HEX(F3, 4)</f>
+        <v>0AB5</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H66" si="2">DEC2BIN(A3,7)</f>
+        <v>0000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A67" si="3">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B67" si="4">B3+0.03082</f>
+        <v>6.164E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D67" si="5">D3+360/75</f>
+        <v>9.6</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.16676874671610226</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>5464.5115236465226</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G67" si="6">DEC2HEX(F4, 4)</f>
+        <v>1558</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="2"/>
+        <v>0000010</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="4"/>
+        <v>9.2460000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="5"/>
+        <v>14.399999999999999</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.24868988716485474</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>8148.8215327307953</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="6"/>
+        <v>1FD4</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>0000011</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5">
+        <f>1/N4</f>
+        <v>2.2727272727272726E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="4"/>
+        <v>0.12328</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="5"/>
+        <v>19.2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.32886664673858323</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>10775.973413683158</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="6"/>
+        <v>2A17</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>0000100</v>
+      </c>
+      <c r="M6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6">
+        <f>N5*1000</f>
+        <v>2.2727272727272725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="4"/>
+        <v>0.15410000000000001</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.40673664307580021</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>13327.539583664746</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="6"/>
+        <v>340F</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v>0000101</v>
+      </c>
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="4"/>
+        <v>0.18492000000000003</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="5"/>
+        <v>28.8</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.48175367410171532</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>15785.622639290907</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="6"/>
+        <v>3DA9</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>0000110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="4"/>
+        <v>0.21574000000000004</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="5"/>
+        <v>33.6</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.55339154924334411</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>18132.980894056655</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="6"/>
+        <v>46D4</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>0000111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="4"/>
+        <v>0.24656000000000006</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="5"/>
+        <v>38.4</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.6211477802783103</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>20353.149316379393</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="6"/>
+        <v>4F81</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>0001000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="4"/>
+        <v>0.27738000000000007</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="5"/>
+        <v>43.199999999999996</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.68454710592868862</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>22430.555019965341</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="6"/>
+        <v>579E</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>0001001</v>
+      </c>
+      <c r="M11">
+        <v>30820</v>
+      </c>
+      <c r="N11">
+        <f>M11*0.000001</f>
+        <v>3.082E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="4"/>
+        <v>0.30820000000000008</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="5"/>
+        <v>47.999999999999993</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.74314482547739413</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>24350.626496417775</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="6"/>
+        <v>5F1E</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>0001010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="4"/>
+        <v>0.3390200000000001</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="5"/>
+        <v>52.79999999999999</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.79652991802419615</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>26099.895823898834</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="6"/>
+        <v>65F3</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>0001011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="4"/>
+        <v>0.36984000000000011</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="5"/>
+        <v>57.599999999999987</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.84432792550201496</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>27666.093134924526</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="6"/>
+        <v>6C12</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>0001100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="4"/>
+        <v>0.40066000000000013</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="5"/>
+        <v>62.399999999999984</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.88620357923121462</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>29038.232680669211</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="6"/>
+        <v>716E</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>0001101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="4"/>
+        <v>0.43148000000000014</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="5"/>
+        <v>67.199999999999989</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.92186315158850052</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>30206.689888100398</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="6"/>
+        <v>75FE</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>0001110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="4"/>
+        <v>0.46230000000000016</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="5"/>
+        <v>71.999999999999986</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.95105651629515353</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>31163.268869443295</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="6"/>
+        <v>79BB</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>0001111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="4"/>
+        <v>0.49312000000000017</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="5"/>
+        <v>76.799999999999983</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.97357890287316018</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>31901.259910444838</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="6"/>
+        <v>7C9D</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>0010000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="4"/>
+        <v>0.52394000000000018</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="5"/>
+        <v>81.59999999999998</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0.98927233296298833</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>32415.48653419824</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="6"/>
+        <v>7E9F</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>0010001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="4"/>
+        <v>0.55476000000000014</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="5"/>
+        <v>86.399999999999977</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.99802672842827156</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>32702.341810409172</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="6"/>
+        <v>7FBE</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>0010010</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="4"/>
+        <v>0.5855800000000001</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="5"/>
+        <v>91.199999999999974</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.9997806834748455</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>32759.813655420261</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="6"/>
+        <v>7FF7</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>0010011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="4"/>
+        <v>0.61640000000000006</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="5"/>
+        <v>95.999999999999972</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0.9945218953682734</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>32587.498945532214</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="6"/>
+        <v>7F4B</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>0010100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="4"/>
+        <v>0.64722000000000002</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="5"/>
+        <v>100.79999999999997</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.98228725072868872</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>32186.606344626944</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="6"/>
+        <v>7DBA</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>0010101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="4"/>
+        <v>0.67803999999999998</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="5"/>
+        <v>105.59999999999997</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.96316256679765833</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>31559.947826258871</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="6"/>
+        <v>7B47</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>0010110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="4"/>
+        <v>0.70885999999999993</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="5"/>
+        <v>110.39999999999996</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.93728198949189179</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>30711.918949680818</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="6"/>
+        <v>77F7</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>0010111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="4"/>
+        <v>0.73967999999999989</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="5"/>
+        <v>115.19999999999996</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0.90482705246601991</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>29648.468028154075</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="6"/>
+        <v>73D0</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>0011000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="4"/>
+        <v>0.77049999999999985</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="5"/>
+        <v>119.99999999999996</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0.86602540378443893</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>28377.054405804709</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="6"/>
+        <v>6ED9</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v>0011001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="4"/>
+        <v>0.80131999999999981</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="5"/>
+        <v>124.79999999999995</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0.82114920913370459</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>26906.5961356841</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="6"/>
+        <v>691A</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>0011010</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="4"/>
+        <v>0.83213999999999977</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="5"/>
+        <v>129.59999999999997</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0.77051324277578948</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>25247.407426034293</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="6"/>
+        <v>629F</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>0011011</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="4"/>
+        <v>0.86295999999999973</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="5"/>
+        <v>134.39999999999998</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0.71447267963280359</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>23411.126293528076</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="6"/>
+        <v>5B73</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>0011100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="4"/>
+        <v>0.89377999999999969</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="5"/>
+        <v>139.19999999999999</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.6534206039901056</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>21410.63293094379</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="6"/>
+        <v>53A2</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>0011101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="4"/>
+        <v>0.92459999999999964</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="5"/>
+        <v>144</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0.58778525229247325</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>19259.95936186747</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="6"/>
+        <v>4B3B</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v>0011110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="4"/>
+        <v>0.9554199999999996</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="5"/>
+        <v>148.80000000000001</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.51802700937313018</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>16974.191016129356</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="6"/>
+        <v>424E</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>0011111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="4"/>
+        <v>0.98623999999999956</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="5"/>
+        <v>153.60000000000002</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0.44463517918492734</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>14569.360916352514</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="6"/>
+        <v>38E9</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v>0100000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="4"/>
+        <v>1.0170599999999996</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="5"/>
+        <v>158.40000000000003</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0.36812455268467731</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>12062.337217818822</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="6"/>
+        <v>2F1E</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v>0100001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="4"/>
+        <v>1.0478799999999997</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="5"/>
+        <v>163.20000000000005</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0.28903179694447084</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>9470.7048904794756</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="6"/>
+        <v>24FE</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="2"/>
+        <v>0100010</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>A36+1</f>
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="4"/>
+        <v>1.0786999999999998</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="5"/>
+        <v>168.00000000000006</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0.20791169081775843</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>6812.6423730254901</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="6"/>
+        <v>1A9C</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="2"/>
+        <v>0100011</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="4"/>
+        <v>1.1095199999999998</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="5"/>
+        <v>172.80000000000007</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0.1253332335643032</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>4106.7940642015228</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="6"/>
+        <v>100A</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="2"/>
+        <v>0100100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="4"/>
+        <v>1.1403399999999999</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="5"/>
+        <v>177.60000000000008</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>4.1875653729198478E-2</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>1372.1395457446465</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="6"/>
+        <v>055C</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="2"/>
+        <v>0100101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="4"/>
+        <v>1.17116</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="5"/>
+        <v>182.40000000000009</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>-4.1875653729201337E-2</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>64161.860454255257</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="6"/>
+        <v>FAA1</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="2"/>
+        <v>0100110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="4"/>
+        <v>1.20198</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="5"/>
+        <v>187.2000000000001</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>-0.12533323356430606</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>61427.205935798382</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="6"/>
+        <v>EFF3</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="2"/>
+        <v>0100111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="4"/>
+        <v>1.2328000000000001</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="5"/>
+        <v>192.00000000000011</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>-0.20791169081776123</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>58721.357626974415</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="6"/>
+        <v>E561</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="2"/>
+        <v>0101000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="4"/>
+        <v>1.2636200000000002</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="5"/>
+        <v>196.80000000000013</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>-0.28903179694447356</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>56063.295109520433</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="6"/>
+        <v>DAFF</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="2"/>
+        <v>0101001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="4"/>
+        <v>1.2944400000000003</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="5"/>
+        <v>201.60000000000014</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>-0.36812455268467997</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>53471.662782181091</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="6"/>
+        <v>D0DF</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="2"/>
+        <v>0101010</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="4"/>
+        <v>1.3252600000000003</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="5"/>
+        <v>206.40000000000015</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>-0.44463517918492995</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>50964.639083647402</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="6"/>
+        <v>C714</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="2"/>
+        <v>0101011</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="4"/>
+        <v>1.3560800000000004</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="5"/>
+        <v>211.20000000000016</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>-0.51802700937313262</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>48559.808983870564</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="6"/>
+        <v>BDAF</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="2"/>
+        <v>0101100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="4"/>
+        <v>1.3869000000000005</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="5"/>
+        <v>216.00000000000017</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>-0.58778525229247558</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>46274.040638132457</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="6"/>
+        <v>B4C2</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="2"/>
+        <v>0101101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="4"/>
+        <v>1.4177200000000005</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="5"/>
+        <v>220.80000000000018</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>-0.65342060399010782</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>44123.367069056141</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="6"/>
+        <v>AC5B</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="2"/>
+        <v>0101110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="4"/>
+        <v>1.4485400000000006</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="5"/>
+        <v>225.60000000000019</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>-0.71447267963280559</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>42122.873706471859</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="6"/>
+        <v>A48A</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="2"/>
+        <v>0101111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="4"/>
+        <v>1.4793600000000007</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="5"/>
+        <v>230.4000000000002</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>-0.77051324277579158</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>40286.592573965638</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="6"/>
+        <v>9D5E</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="2"/>
+        <v>0110000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="4"/>
+        <v>1.5101800000000007</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="5"/>
+        <v>235.20000000000022</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>-0.82114920913370626</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>38627.403864315842</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="6"/>
+        <v>96E3</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="2"/>
+        <v>0110001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="4"/>
+        <v>1.5410000000000008</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="5"/>
+        <v>240.00000000000023</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>-0.86602540378444059</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>37156.945594195233</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="6"/>
+        <v>9124</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="2"/>
+        <v>0110010</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="4"/>
+        <v>1.5718200000000009</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="5"/>
+        <v>244.80000000000024</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>-0.90482705246602124</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>35885.531971845878</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="6"/>
+        <v>8C2D</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="2"/>
+        <v>0110011</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="4"/>
+        <v>1.602640000000001</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="5"/>
+        <v>249.60000000000025</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>-0.93728198949189301</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>34822.081050319146</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="6"/>
+        <v>8806</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="2"/>
+        <v>0110100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="4"/>
+        <v>1.633460000000001</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="5"/>
+        <v>254.40000000000026</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>-0.96316256679765933</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>33974.052173741096</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="6"/>
+        <v>84B6</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="2"/>
+        <v>0110101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="4"/>
+        <v>1.6642800000000011</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="5"/>
+        <v>259.20000000000027</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>-0.9822872507286895</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>33347.393655373031</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="6"/>
+        <v>8243</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="2"/>
+        <v>0110110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="4"/>
+        <v>1.6951000000000012</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="5"/>
+        <v>264.00000000000028</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>-0.99452189536827384</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>32946.501054467772</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="6"/>
+        <v>80B2</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="2"/>
+        <v>0110111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="4"/>
+        <v>1.7259200000000012</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="5"/>
+        <v>268.8000000000003</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>-0.99978068347484561</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>32774.186344579735</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="6"/>
+        <v>8006</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="2"/>
+        <v>0111000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="4"/>
+        <v>1.7567400000000013</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="5"/>
+        <v>273.60000000000031</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>-0.99802672842827123</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>32831.658189590838</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="6"/>
+        <v>803F</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="2"/>
+        <v>0111001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="4"/>
+        <v>1.7875600000000014</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="5"/>
+        <v>278.40000000000032</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>-0.98927233296298744</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>33118.513465801792</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="6"/>
+        <v>815E</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="2"/>
+        <v>0111010</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="4"/>
+        <v>1.8183800000000014</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="5"/>
+        <v>283.20000000000033</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>-0.97357890287315896</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>33632.740089555198</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="6"/>
+        <v>8360</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="2"/>
+        <v>0111011</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="4"/>
+        <v>1.8492000000000015</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="5"/>
+        <v>288.00000000000034</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="0"/>
+        <v>-0.95105651629515175</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>34370.731130556764</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="6"/>
+        <v>8642</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="2"/>
+        <v>0111100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="4"/>
+        <v>1.8800200000000016</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="5"/>
+        <v>292.80000000000035</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="0"/>
+        <v>-0.92186315158849819</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>35327.310111899678</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="6"/>
+        <v>89FF</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="2"/>
+        <v>0111101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="4"/>
+        <v>1.9108400000000016</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="5"/>
+        <v>297.60000000000036</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>-0.88620357923121185</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>36495.76731933088</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="6"/>
+        <v>8E8F</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="2"/>
+        <v>0111110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="4"/>
+        <v>1.9416600000000017</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="5"/>
+        <v>302.40000000000038</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="0"/>
+        <v>-0.84432792550201163</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>37867.90686507558</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="6"/>
+        <v>93EB</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="2"/>
+        <v>0111111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="4"/>
+        <v>1.9724800000000018</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="5"/>
+        <v>307.20000000000039</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="0"/>
+        <v>-0.79652991802419237</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>39434.104176101289</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="6"/>
+        <v>9A0A</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="2"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="4"/>
+        <v>2.0033000000000016</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="5"/>
+        <v>312.0000000000004</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E111" si="7">SIN(RADIANS(D67))</f>
+        <v>-0.7431448254773898</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F111" si="8">IF(E67&gt;=0, E67*32767, E67*32767+32767*2)</f>
+        <v>41183.373503582363</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="6"/>
+        <v>A0DF</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" ref="H67:H111" si="9">DEC2BIN(A67,7)</f>
+        <v>1000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" ref="A68:A111" si="10">A67+1</f>
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <f t="shared" ref="B68:B104" si="11">B67+0.03082</f>
+        <v>2.0341200000000015</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ref="D68:D77" si="12">D67+360/75</f>
+        <v>316.80000000000041</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="7"/>
+        <v>-0.68454710592868373</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="8"/>
+        <v>43103.444980034823</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" ref="G68:G111" si="13">DEC2HEX(F68, 4)</f>
+        <v>A85F</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="9"/>
+        <v>1000010</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="10"/>
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="11"/>
+        <v>2.0649400000000013</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="12"/>
+        <v>321.60000000000042</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="7"/>
+        <v>-0.62114778027830497</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="8"/>
+        <v>45180.850683620782</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="13"/>
+        <v>B07C</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="9"/>
+        <v>1000011</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="10"/>
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="11"/>
+        <v>2.0957600000000012</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="12"/>
+        <v>326.40000000000043</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="7"/>
+        <v>-0.55339154924333755</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="8"/>
+        <v>47401.01910594356</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="13"/>
+        <v>B929</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="9"/>
+        <v>1000100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="10"/>
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="11"/>
+        <v>2.126580000000001</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="12"/>
+        <v>331.20000000000044</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="7"/>
+        <v>-0.48175367410170833</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="8"/>
+        <v>49748.377360709324</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="13"/>
+        <v>C254</v>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" si="9"/>
+        <v>1000101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="10"/>
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="11"/>
+        <v>2.1574000000000009</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="12"/>
+        <v>336.00000000000045</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="7"/>
+        <v>-0.40673664307579283</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="8"/>
+        <v>52206.460416335496</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="13"/>
+        <v>CBEE</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="9"/>
+        <v>1000110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="10"/>
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="11"/>
+        <v>2.1882200000000007</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="12"/>
+        <v>340.80000000000047</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="7"/>
+        <v>-0.32886664673857552</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="8"/>
+        <v>54758.026586317093</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="13"/>
+        <v>D5E6</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="9"/>
+        <v>1000111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="10"/>
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="11"/>
+        <v>2.2190400000000006</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="12"/>
+        <v>345.60000000000048</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="7"/>
+        <v>-0.24868988716484675</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="8"/>
+        <v>57385.178467269463</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="13"/>
+        <v>E029</v>
+      </c>
+      <c r="H74" t="str">
+        <f t="shared" si="9"/>
+        <v>1001000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="10"/>
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="11"/>
+        <v>2.2498600000000004</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="12"/>
+        <v>350.40000000000049</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="7"/>
+        <v>-0.16676874671609399</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="8"/>
+        <v>60069.488476353748</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="13"/>
+        <v>EAA5</v>
+      </c>
+      <c r="H75" t="str">
+        <f t="shared" si="9"/>
+        <v>1001001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="10"/>
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="11"/>
+        <v>2.2806800000000003</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="12"/>
+        <v>355.2000000000005</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="7"/>
+        <v>-8.3677843332307003E-2</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="8"/>
+        <v>62792.128107530298</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="13"/>
+        <v>F548</v>
+      </c>
+      <c r="H76" t="str">
+        <f t="shared" si="9"/>
+        <v>1001010</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="10"/>
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="11"/>
+        <v>2.3115000000000001</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="12"/>
+        <v>360.00000000000051</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="7"/>
+        <v>8.6367545060195283E-15</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="8"/>
+        <v>2.8300053489874188E-10</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="13"/>
+        <v>0000</v>
+      </c>
+      <c r="H77" t="str">
+        <f t="shared" si="9"/>
+        <v>1001011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N94"/>
   <sheetViews>
@@ -13940,7 +16311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N75"/>
   <sheetViews>
@@ -16237,7 +18608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H111"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added E5 file for testing
</commit_message>
<xml_diff>
--- a/Wave Math/Tone_calculator.xlsx
+++ b/Wave Math/Tone_calculator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="6795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="6795" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Base tone" sheetId="1" r:id="rId1"/>
@@ -3132,8 +3132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="C20" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12370,10 +12370,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12465,11 +12465,11 @@
         <v>0.127877161684506</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F50" si="1">IF(E3&gt;=0, E3*32767, E3*32767+32767*2)</f>
+        <f t="shared" ref="F3:F66" si="1">IF(E3&gt;=0, E3*32767, E3*32767+32767*2)</f>
         <v>4190.1509569162081</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G50" si="2">DEC2HEX(F3,4)</f>
+        <f t="shared" ref="G3:G66" si="2">DEC2HEX(F3,4)</f>
         <v>105E</v>
       </c>
       <c r="H3" t="str">
@@ -12479,15 +12479,15 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A50" si="4">A3+1</f>
+        <f t="shared" ref="A4:A67" si="4">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B51" si="5">B3+0.03082</f>
+        <f t="shared" ref="B4:B67" si="5">B3+0.03082</f>
         <v>6.164E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D51" si="6">D3+360/49</f>
+        <f t="shared" ref="D4:D67" si="6">D3+360/49</f>
         <v>14.693877551020408</v>
       </c>
       <c r="E4">
@@ -13908,6 +13908,755 @@
       <c r="H50" t="str">
         <f t="shared" si="3"/>
         <v>0110000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="5"/>
+        <v>1.5101800000000007</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <f t="shared" ref="E51:E74" si="7">SIN(RADIANS(D51))</f>
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <f t="shared" ref="F51:F74" si="8">IF(E51&gt;=0, E51*32767, E51*32767+32767*2)</f>
+        <v>0</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="2"/>
+        <v>0000</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" ref="H51:H74" si="9">DEC2BIN(A51, 7)</f>
+        <v>0110001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="5"/>
+        <v>1.5410000000000008</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="6"/>
+        <v>7.3469387755102042</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="7"/>
+        <v>0.127877161684506</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="8"/>
+        <v>4190.1509569162081</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="2"/>
+        <v>105E</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="9"/>
+        <v>0110010</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="5"/>
+        <v>1.5718200000000009</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="6"/>
+        <v>14.693877551020408</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="7"/>
+        <v>0.25365458390950735</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="8"/>
+        <v>8311.4997509628265</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="2"/>
+        <v>2077</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="9"/>
+        <v>0110011</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="4"/>
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="5"/>
+        <v>1.602640000000001</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="6"/>
+        <v>22.040816326530614</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="7"/>
+        <v>0.37526700487937414</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="8"/>
+        <v>12296.373948882452</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="2"/>
+        <v>3008</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="9"/>
+        <v>0110100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="5"/>
+        <v>1.633460000000001</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="6"/>
+        <v>29.387755102040817</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="7"/>
+        <v>0.49071755200393785</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="8"/>
+        <v>16079.342026513032</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="2"/>
+        <v>3ECF</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="9"/>
+        <v>0110101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="5"/>
+        <v>1.6642800000000011</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="6"/>
+        <v>36.734693877551024</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="7"/>
+        <v>0.5981105304912161</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="8"/>
+        <v>19598.287752605676</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="2"/>
+        <v>4C8E</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="9"/>
+        <v>0110110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="5"/>
+        <v>1.6951000000000012</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="6"/>
+        <v>44.081632653061227</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="7"/>
+        <v>0.69568255060348638</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="8"/>
+        <v>22795.43013562444</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="2"/>
+        <v>590B</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="9"/>
+        <v>0110111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="5"/>
+        <v>1.7259200000000012</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="6"/>
+        <v>51.428571428571431</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="7"/>
+        <v>0.7818314824680298</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="8"/>
+        <v>25618.272186029932</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="2"/>
+        <v>6412</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="9"/>
+        <v>0111000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="5"/>
+        <v>1.7567400000000013</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="6"/>
+        <v>58.775510204081634</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="7"/>
+        <v>0.85514276300534608</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="8"/>
+        <v>28020.462915396176</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="2"/>
+        <v>6D74</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="9"/>
+        <v>0111001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="5"/>
+        <v>1.7875600000000014</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="6"/>
+        <v>66.122448979591837</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="7"/>
+        <v>0.9144126230158125</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="8"/>
+        <v>29962.558418359127</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="2"/>
+        <v>750A</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="9"/>
+        <v>0111010</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="5"/>
+        <v>1.8183800000000014</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="6"/>
+        <v>73.469387755102048</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="7"/>
+        <v>0.95866785303666069</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="8"/>
+        <v>31412.669540452262</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="2"/>
+        <v>7AB4</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="9"/>
+        <v>0111011</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="5"/>
+        <v>1.8492000000000015</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="6"/>
+        <v>80.816326530612258</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="7"/>
+        <v>0.98718178341445018</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="8"/>
+        <v>32346.98549714129</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="2"/>
+        <v>7E5A</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="9"/>
+        <v>0111100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="4"/>
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="5"/>
+        <v>1.8800200000000016</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="6"/>
+        <v>88.163265306122469</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="7"/>
+        <v>0.99948621620068789</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="8"/>
+        <v>32750.164846247939</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="2"/>
+        <v>7FEE</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="9"/>
+        <v>0111101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="4"/>
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="5"/>
+        <v>1.9108400000000016</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="6"/>
+        <v>95.510204081632679</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="7"/>
+        <v>0.99537911294919812</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="8"/>
+        <v>32615.587394006376</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="2"/>
+        <v>7F67</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="9"/>
+        <v>0111110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="5"/>
+        <v>1.9416600000000017</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="6"/>
+        <v>102.85714285714289</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="7"/>
+        <v>0.97492791218182351</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="8"/>
+        <v>31945.46289846181</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="2"/>
+        <v>7CC9</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="9"/>
+        <v>0111111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="5"/>
+        <v>1.9724800000000018</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="6"/>
+        <v>110.2040816326531</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="7"/>
+        <v>0.93846842204976011</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="8"/>
+        <v>30750.79478530449</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="2"/>
+        <v>781E</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="9"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="5"/>
+        <v>2.0033000000000016</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="6"/>
+        <v>117.55102040816331</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="7"/>
+        <v>0.88659930637299977</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="8"/>
+        <v>29051.199471924083</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" ref="G67:G76" si="10">DEC2HEX(F67,4)</f>
+        <v>717B</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="9"/>
+        <v>1000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" ref="A68:A76" si="11">A67+1</f>
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <f t="shared" ref="B68:B76" si="12">B67+0.03082</f>
+        <v>2.0341200000000015</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ref="D68:D76" si="13">D67+360/49</f>
+        <v>124.89795918367352</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="7"/>
+        <v>0.82017225459695531</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="8"/>
+        <v>26874.584266378435</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="10"/>
+        <v>68FA</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="9"/>
+        <v>1000010</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="11"/>
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="12"/>
+        <v>2.0649400000000013</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="13"/>
+        <v>132.24489795918373</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="7"/>
+        <v>0.74027799707531483</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="8"/>
+        <v>24256.68913016684</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="10"/>
+        <v>5EC0</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="9"/>
+        <v>1000011</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="11"/>
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="12"/>
+        <v>2.0957600000000012</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="13"/>
+        <v>139.59183673469394</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="7"/>
+        <v>0.64822839530778775</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="8"/>
+        <v>21240.499829050281</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="10"/>
+        <v>52F8</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="9"/>
+        <v>1000100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="11"/>
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="12"/>
+        <v>2.126580000000001</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="13"/>
+        <v>146.93877551020415</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="7"/>
+        <v>0.5455349012105476</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="8"/>
+        <v>17875.542107966012</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="10"/>
+        <v>45D3</v>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" si="9"/>
+        <v>1000101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="11"/>
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="12"/>
+        <v>2.1574000000000009</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="13"/>
+        <v>154.28571428571436</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="7"/>
+        <v>0.43388373911755701</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="8"/>
+        <v>14217.068479664991</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="10"/>
+        <v>3789</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="9"/>
+        <v>1000110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="11"/>
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="12"/>
+        <v>2.1882200000000007</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="13"/>
+        <v>161.63265306122457</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="7"/>
+        <v>0.31510821802361916</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="8"/>
+        <v>10325.15097997993</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="10"/>
+        <v>2855</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="9"/>
+        <v>1000111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="11"/>
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="12"/>
+        <v>2.2190400000000006</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="13"/>
+        <v>168.97959183673478</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="7"/>
+        <v>0.19115862870137079</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="8"/>
+        <v>6263.6947866578166</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="10"/>
+        <v>1877</v>
+      </c>
+      <c r="H74" t="str">
+        <f t="shared" si="9"/>
+        <v>1001000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="11"/>
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="12"/>
+        <v>2.2498600000000004</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="13"/>
+        <v>176.32653061224499</v>
+      </c>
+      <c r="E75">
+        <f t="shared" ref="E75:E76" si="14">SIN(RADIANS(D75))</f>
+        <v>6.4070219980711454E-2</v>
+      </c>
+      <c r="F75">
+        <f t="shared" ref="F75:F76" si="15">IF(E75&gt;=0, E75*32767, E75*32767+32767*2)</f>
+        <v>2099.3888981079722</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="10"/>
+        <v>0833</v>
+      </c>
+      <c r="H75" t="str">
+        <f t="shared" ref="H75:H76" si="16">DEC2BIN(A75, 7)</f>
+        <v>1001001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>